<commit_message>
Filename fix and adjustment to calculation of real cost of capital
</commit_message>
<xml_diff>
--- a/InputData/indst/BCoISC/BAU Cost of Industry Sector Capital.xlsx
+++ b/InputData/indst/BCoISC/BAU Cost of Industry Sector Capital.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\indst\BCoISC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB6A2B2-64B4-42EE-8A0D-1CDEDD183566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41863536-2C69-4524-8252-E8C88DBF4DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58815" yWindow="1905" windowWidth="24720" windowHeight="13710" xr2:uid="{C8F9D547-902B-4E49-8BA2-E23B0A2DC1A9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C8F9D547-902B-4E49-8BA2-E23B0A2DC1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="NYU Data" sheetId="7" r:id="rId2"/>
     <sheet name="EPS &lt;&gt; NYU Industry Mapping" sheetId="8" r:id="rId3"/>
-    <sheet name="BCoESC-WACCbI" sheetId="3" r:id="rId4"/>
-    <sheet name="BCoESC-RPfE" sheetId="4" r:id="rId5"/>
+    <sheet name="BCoISC-WACCbI" sheetId="3" r:id="rId4"/>
+    <sheet name="BCoISC-RPfE" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="194">
   <si>
     <t>Source:</t>
   </si>
@@ -590,12 +590,6 @@
     <t>Weighted Average Cost of Capital</t>
   </si>
   <si>
-    <t>BCoESC-RPfE  Risk Premium for Equity</t>
-  </si>
-  <si>
-    <t>BCoESC-WACCbI  Weighted Average Cost of Capital by Industry</t>
-  </si>
-  <si>
     <t>Cost of Capital for Industry Sector Projects</t>
   </si>
   <si>
@@ -618,6 +612,59 @@
   </si>
   <si>
     <t>We use the nominal WACC from NYU then adjust it by inflation.</t>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>real</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = (1 + r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/(1 + i) - 1</t>
+    </r>
+  </si>
+  <si>
+    <t>BCoISC-WACCbI  Weighted Average Cost of Capital by Industry</t>
+  </si>
+  <si>
+    <t>BCoISC-RPfE  Risk Premium for Equity</t>
   </si>
 </sst>
 </file>
@@ -627,7 +674,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,6 +800,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2078,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F0629E-7DF7-4E6A-B1DA-78D3050B5FAD}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2091,12 +2146,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2107,12 +2162,12 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2127,12 +2182,12 @@
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2142,7 +2197,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2157,12 +2212,12 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2194,7 +2249,12 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16.5">
+      <c r="A25" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2210,7 +2270,7 @@
   <dimension ref="A1:L115"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -7633,7 +7693,7 @@
   <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K27"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8321,7 +8381,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8357,8 +8417,8 @@
         <v>147</v>
       </c>
       <c r="B2" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K3-'NYU Data'!C$17</f>
-        <v>4.9333757172636876E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K3)/(1+'NYU Data'!C$17)-1</f>
+        <v>4.8130494802572477E-2</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -8366,8 +8426,8 @@
         <v>148</v>
       </c>
       <c r="B3" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K4-'NYU Data'!C$17</f>
-        <v>6.7344036982938393E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K4)/(1+'NYU Data'!C$17)-1</f>
+        <v>6.570149949554982E-2</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -8375,8 +8435,8 @@
         <v>149</v>
       </c>
       <c r="B4" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K5-'NYU Data'!C$17</f>
-        <v>5.0232173387922262E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K5)/(1+'NYU Data'!C$17)-1</f>
+        <v>4.9006998427241211E-2</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -8384,8 +8444,8 @@
         <v>150</v>
       </c>
       <c r="B5" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K6-'NYU Data'!C$17</f>
-        <v>5.9036298078024345E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K6)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.7596388368804208E-2</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -8393,8 +8453,8 @@
         <v>151</v>
       </c>
       <c r="B6" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K7-'NYU Data'!C$17</f>
-        <v>4.3678670784462158E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K7)/(1+'NYU Data'!C$17)-1</f>
+        <v>4.2613337350694946E-2</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -8402,8 +8462,8 @@
         <v>152</v>
       </c>
       <c r="B7" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K8-'NYU Data'!C$17</f>
-        <v>4.9429651061627063E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K8)/(1+'NYU Data'!C$17)-1</f>
+        <v>4.8224049816221637E-2</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -8411,8 +8471,8 @@
         <v>153</v>
       </c>
       <c r="B8" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K9-'NYU Data'!C$17</f>
-        <v>5.8211276108504302E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K9)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.6791488886345665E-2</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -8420,8 +8480,8 @@
         <v>154</v>
       </c>
       <c r="B9" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K10-'NYU Data'!C$17</f>
-        <v>4.9745489154480564E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K10)/(1+'NYU Data'!C$17)-1</f>
+        <v>4.8532184540956758E-2</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -8429,8 +8489,8 @@
         <v>155</v>
       </c>
       <c r="B10" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K11-'NYU Data'!C$17</f>
-        <v>3.8289396315035591E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K11)/(1+'NYU Data'!C$17)-1</f>
+        <v>3.7355508600034781E-2</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -8438,8 +8498,8 @@
         <v>156</v>
       </c>
       <c r="B11" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K12-'NYU Data'!C$17</f>
-        <v>4.7554664806010082E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K12)/(1+'NYU Data'!C$17)-1</f>
+        <v>4.6394794932692829E-2</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -8447,8 +8507,8 @@
         <v>157</v>
       </c>
       <c r="B12" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K13-'NYU Data'!C$17</f>
-        <v>2.8344322604215551E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K13)/(1+'NYU Data'!C$17)-1</f>
+        <v>2.7652997662649392E-2</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -8456,8 +8516,8 @@
         <v>158</v>
       </c>
       <c r="B13" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K14-'NYU Data'!C$17</f>
-        <v>6.9602959728378599E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K14)/(1+'NYU Data'!C$17)-1</f>
+        <v>6.7905326564271951E-2</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -8465,8 +8525,8 @@
         <v>159</v>
       </c>
       <c r="B14" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K15-'NYU Data'!C$17</f>
-        <v>6.9602959728378599E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K15)/(1+'NYU Data'!C$17)-1</f>
+        <v>6.7905326564271951E-2</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -8474,8 +8534,8 @@
         <v>160</v>
       </c>
       <c r="B15" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K16-'NYU Data'!C$17</f>
-        <v>5.6745309550233956E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K16)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.5361277609984549E-2</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -8483,8 +8543,8 @@
         <v>161</v>
       </c>
       <c r="B16" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K17-'NYU Data'!C$17</f>
-        <v>5.9036298078024345E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K17)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.7596388368804208E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -8492,8 +8552,8 @@
         <v>162</v>
       </c>
       <c r="B17" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K18-'NYU Data'!C$17</f>
-        <v>5.9036298078024345E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K18)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.7596388368804208E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -8501,8 +8561,8 @@
         <v>163</v>
       </c>
       <c r="B18" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K19-'NYU Data'!C$17</f>
-        <v>5.8374032727640197E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K19)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.695027583184431E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -8510,8 +8570,8 @@
         <v>164</v>
       </c>
       <c r="B19" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K20-'NYU Data'!C$17</f>
-        <v>5.7735480310145602E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K20)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.6327297863556725E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -8519,8 +8579,8 @@
         <v>165</v>
       </c>
       <c r="B20" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K21-'NYU Data'!C$17</f>
-        <v>6.0408807318036419E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K21)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.8935421773694152E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -8528,8 +8588,8 @@
         <v>166</v>
       </c>
       <c r="B21" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K22-'NYU Data'!C$17</f>
-        <v>5.5543293741726181E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K22)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.4188579260220582E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -8537,8 +8597,8 @@
         <v>167</v>
       </c>
       <c r="B22" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K23-'NYU Data'!C$17</f>
-        <v>5.2547297393384491E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K23)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.1265655993545822E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -8546,8 +8606,8 @@
         <v>168</v>
       </c>
       <c r="B23" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K24-'NYU Data'!C$17</f>
-        <v>6.0408807318036419E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K24)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.8935421773694152E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -8555,8 +8615,8 @@
         <v>169</v>
       </c>
       <c r="B24" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K25-'NYU Data'!C$17</f>
-        <v>4.0893802487895418E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K25)/(1+'NYU Data'!C$17)-1</f>
+        <v>3.9896392671117553E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -8564,8 +8624,8 @@
         <v>170</v>
       </c>
       <c r="B25" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K26-'NYU Data'!C$17</f>
-        <v>3.6475037186992132E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K26)/(1+'NYU Data'!C$17)-1</f>
+        <v>3.5585402133651023E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -8573,8 +8633,8 @@
         <v>171</v>
       </c>
       <c r="B26" s="9">
-        <f>'EPS &lt;&gt; NYU Industry Mapping'!K27-'NYU Data'!C$17</f>
-        <v>5.6702673363264199E-2</v>
+        <f>(1+'EPS &lt;&gt; NYU Industry Mapping'!K27)/(1+'NYU Data'!C$17)-1</f>
+        <v>5.5319681330013859E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8590,7 +8650,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>